<commit_message>
Add several more submissions
Naive Bayes and SVM models were cross-validated. Naive Bayes and neural network (one layer, 50% dropout) were tested, though neither did as well as logistic regression. Sentiment scores added another feature, but they did not lead to any increase in the final score when used in the logistic model. The whole file was cleaned up and organized into sections.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zuloo\Desktop\Syracuse Data Science\Semester 3\IST 707\Homework\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zuloo\Desktop\SeanScripts\nlp-getting-started\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D420D49-34FB-4852-B227-42D2FADC0109}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A7751E-E7EE-4030-A913-2462BE81CACD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="33">
   <si>
     <t>Model</t>
   </si>
@@ -99,19 +99,37 @@
     <t>Reason</t>
   </si>
   <si>
-    <t>Highest F random forest</t>
-  </si>
-  <si>
     <t>Best model</t>
   </si>
   <si>
     <t>Comparison with preprocessing</t>
   </si>
   <si>
-    <t>Second best model</t>
-  </si>
-  <si>
     <t>Highest recall? Probably not worth submitting</t>
+  </si>
+  <si>
+    <t>Linear SVM</t>
+  </si>
+  <si>
+    <t>Multinomial NB</t>
+  </si>
+  <si>
+    <t>Best random forest</t>
+  </si>
+  <si>
+    <t>Neural Network</t>
+  </si>
+  <si>
+    <t>Best SVM</t>
+  </si>
+  <si>
+    <t>Best neural net</t>
+  </si>
+  <si>
+    <t>Seeing if bigrams helped in the final result</t>
+  </si>
+  <si>
+    <t>Best NB</t>
   </si>
 </sst>
 </file>
@@ -161,11 +179,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,15 +466,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="F45" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="12" width="11.85546875" customWidth="1"/>
   </cols>
@@ -539,7 +558,7 @@
         <v>0.79549999999999998</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -600,7 +619,7 @@
       <c r="G4" s="2">
         <v>1.46E-2</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="4">
         <v>0.91620000000000001</v>
       </c>
       <c r="I4" s="2">
@@ -613,9 +632,6 @@
         <v>9.4000000000000004E-3</v>
       </c>
       <c r="L4" s="2"/>
-      <c r="M4" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -727,7 +743,7 @@
         <v>0.78732000000000002</v>
       </c>
       <c r="M7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -984,7 +1000,7 @@
         <v>0.80979999999999996</v>
       </c>
       <c r="M14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1169,7 +1185,7 @@
         <v>0.78220000000000001</v>
       </c>
       <c r="M19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1318,7 +1334,7 @@
         <v>0.79549999999999998</v>
       </c>
       <c r="M23" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1391,7 +1407,1395 @@
         <v>9.7000000000000003E-3</v>
       </c>
     </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.80610000000000004</v>
+      </c>
+      <c r="E26" s="1">
+        <v>6.6E-3</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.79769999999999996</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.88439999999999996</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.8387</v>
+      </c>
+      <c r="K26" s="1">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0.80269999999999997</v>
+      </c>
+      <c r="M26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="E27" s="1">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.78620000000000001</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2.18E-2</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.87780000000000002</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.82930000000000004</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.79769999999999996</v>
+      </c>
+      <c r="E28" s="1">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.78959999999999997</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1.9300000000000001E-2</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.87970000000000004</v>
+      </c>
+      <c r="I28" s="1">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0.83220000000000005</v>
+      </c>
+      <c r="K28" s="1">
+        <v>9.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.80069999999999997</v>
+      </c>
+      <c r="E29" s="1">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.79010000000000002</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.88660000000000005</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.83530000000000004</v>
+      </c>
+      <c r="K29" s="1">
+        <v>6.6E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.78710000000000002</v>
+      </c>
+      <c r="E30" s="1">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.7883</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.85670000000000002</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="K30" s="1">
+        <v>9.7000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.7863</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.79210000000000003</v>
+      </c>
+      <c r="G31" s="1">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.8478</v>
+      </c>
+      <c r="I31" s="1">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.81889999999999996</v>
+      </c>
+      <c r="K31" s="1">
+        <v>4.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.80049999999999999</v>
+      </c>
+      <c r="E32" s="1">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0.7944</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0.87760000000000005</v>
+      </c>
+      <c r="I32" s="1">
+        <v>1.84E-2</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0.8337</v>
+      </c>
+      <c r="K32" s="1">
+        <v>8.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.79079999999999995</v>
+      </c>
+      <c r="E33" s="1">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.78539999999999999</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1.95E-2</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0.87129999999999996</v>
+      </c>
+      <c r="I33" s="1">
+        <v>1.21E-2</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="K33" s="1">
+        <v>9.4999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.79110000000000003</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1.12E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.78290000000000004</v>
+      </c>
+      <c r="G34" s="1">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0.877</v>
+      </c>
+      <c r="I34" s="1">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0.82720000000000005</v>
+      </c>
+      <c r="K34" s="1">
+        <v>1.2200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.80630000000000002</v>
+      </c>
+      <c r="E35" s="1">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.80020000000000002</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1.49E-2</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="I35" s="1">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0.83809999999999996</v>
+      </c>
+      <c r="K35" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.79530000000000001</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1.14E-2</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0.78590000000000004</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.88170000000000004</v>
+      </c>
+      <c r="I36" s="1">
+        <v>1.24E-2</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0.83089999999999997</v>
+      </c>
+      <c r="K36" s="1">
+        <v>1.0699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.7944</v>
+      </c>
+      <c r="E37" s="1">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.78790000000000004</v>
+      </c>
+      <c r="G37" s="1">
+        <v>2.29E-2</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.87570000000000003</v>
+      </c>
+      <c r="I37" s="1">
+        <v>1.78E-2</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0.82930000000000004</v>
+      </c>
+      <c r="K37" s="1">
+        <v>9.5999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.80359999999999998</v>
+      </c>
+      <c r="E38" s="2">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.79330000000000001</v>
+      </c>
+      <c r="G38" s="2">
+        <v>1.43E-2</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.88670000000000004</v>
+      </c>
+      <c r="I38" s="2">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0.83730000000000004</v>
+      </c>
+      <c r="K38" s="2">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="L38" s="2">
+        <v>0.79344999999999999</v>
+      </c>
+      <c r="M38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.68620000000000003</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.65790000000000004</v>
+      </c>
+      <c r="G39" s="2">
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0.93740000000000001</v>
+      </c>
+      <c r="I39" s="2">
+        <v>1.29E-2</v>
+      </c>
+      <c r="J39" s="2">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="K39" s="2">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.75670000000000004</v>
+      </c>
+      <c r="E40" s="2">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.71430000000000005</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0.95579999999999998</v>
+      </c>
+      <c r="I40" s="2">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0.8175</v>
+      </c>
+      <c r="K40" s="2">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.79879999999999995</v>
+      </c>
+      <c r="E41" s="2">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.7802</v>
+      </c>
+      <c r="G41" s="2">
+        <v>1.47E-2</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="I41" s="2">
+        <v>1.03E-2</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0.83620000000000005</v>
+      </c>
+      <c r="K41" s="2">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.67110000000000003</v>
+      </c>
+      <c r="E42" s="2">
+        <v>3.1600000000000003E-2</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.64029999999999998</v>
+      </c>
+      <c r="G42" s="2">
+        <v>3.0800000000000001E-2</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="I42" s="2">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="J42" s="2">
+        <v>0.77049999999999996</v>
+      </c>
+      <c r="K42" s="2">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1.14E-2</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.75319999999999998</v>
+      </c>
+      <c r="G43" s="2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.89539999999999997</v>
+      </c>
+      <c r="I43" s="2">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="J43" s="2">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="K43" s="2">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.79810000000000003</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.78910000000000002</v>
+      </c>
+      <c r="G44" s="2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0.88170000000000004</v>
+      </c>
+      <c r="I44" s="2">
+        <v>1.21E-2</v>
+      </c>
+      <c r="J44" s="2">
+        <v>0.83279999999999998</v>
+      </c>
+      <c r="K44" s="2">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.66169999999999995</v>
+      </c>
+      <c r="G45" s="2">
+        <v>2.24E-2</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0.89510000000000001</v>
+      </c>
+      <c r="I45" s="2">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="J45" s="2">
+        <v>0.76070000000000004</v>
+      </c>
+      <c r="K45" s="2">
+        <v>1.43E-2</v>
+      </c>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.75580000000000003</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1.24E-2</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.71660000000000001</v>
+      </c>
+      <c r="G46" s="2">
+        <v>1.89E-2</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="I46" s="2">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="J46" s="2">
+        <v>0.81540000000000001</v>
+      </c>
+      <c r="K46" s="2">
+        <v>1.14E-2</v>
+      </c>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.8014</v>
+      </c>
+      <c r="E47" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.79169999999999996</v>
+      </c>
+      <c r="G47" s="2">
+        <v>1.37E-2</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0.88439999999999996</v>
+      </c>
+      <c r="I47" s="2">
+        <v>8.6E-3</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0.83540000000000003</v>
+      </c>
+      <c r="K47" s="2">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.6905</v>
+      </c>
+      <c r="E48" s="2">
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.6633</v>
+      </c>
+      <c r="G48" s="2">
+        <v>2.29E-2</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0.92910000000000004</v>
+      </c>
+      <c r="I48" s="2">
+        <v>1.67E-2</v>
+      </c>
+      <c r="J48" s="2">
+        <v>0.77390000000000003</v>
+      </c>
+      <c r="K48" s="2">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.75949999999999995</v>
+      </c>
+      <c r="E49" s="2">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.72019999999999995</v>
+      </c>
+      <c r="G49" s="2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0.94569999999999999</v>
+      </c>
+      <c r="I49" s="2">
+        <v>6.6E-3</v>
+      </c>
+      <c r="J49" s="2">
+        <v>0.81759999999999999</v>
+      </c>
+      <c r="K49" s="2">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.79559999999999997</v>
+      </c>
+      <c r="E50" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.79310000000000003</v>
+      </c>
+      <c r="G50" s="2">
+        <v>1.54E-2</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="I50" s="2">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="J50" s="2">
+        <v>0.82879999999999998</v>
+      </c>
+      <c r="K50" s="2">
+        <v>9.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E51" s="2">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.65769999999999995</v>
+      </c>
+      <c r="G51" s="2">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0.98850000000000005</v>
+      </c>
+      <c r="I51" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J51" s="2">
+        <v>0.78979999999999995</v>
+      </c>
+      <c r="K51" s="2">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="M51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.78339999999999999</v>
+      </c>
+      <c r="E52" s="2">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.74639999999999995</v>
+      </c>
+      <c r="G52" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0.93930000000000002</v>
+      </c>
+      <c r="I52" s="2">
+        <v>1.23E-2</v>
+      </c>
+      <c r="J52" s="2">
+        <v>0.83169999999999999</v>
+      </c>
+      <c r="K52" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.79269999999999996</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.79410000000000003</v>
+      </c>
+      <c r="G53" s="2">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0.8589</v>
+      </c>
+      <c r="I53" s="2">
+        <v>1.12E-2</v>
+      </c>
+      <c r="J53" s="2">
+        <v>0.82520000000000004</v>
+      </c>
+      <c r="K53" s="2">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.77180000000000004</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1.67E-2</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0.74019999999999997</v>
+      </c>
+      <c r="G54" s="2">
+        <v>2.3099999999999999E-2</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0.9244</v>
+      </c>
+      <c r="I54" s="2">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="J54" s="2">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="K54" s="2">
+        <v>1.47E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.78690000000000004</v>
+      </c>
+      <c r="E55" s="2">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0.79210000000000003</v>
+      </c>
+      <c r="G55" s="2">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="H55" s="2">
+        <v>0.84909999999999997</v>
+      </c>
+      <c r="I55" s="2">
+        <v>1.35E-2</v>
+      </c>
+      <c r="J55" s="2">
+        <v>0.8196</v>
+      </c>
+      <c r="K55" s="2">
+        <v>1.0800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.78720000000000001</v>
+      </c>
+      <c r="E56" s="2">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.78869999999999996</v>
+      </c>
+      <c r="G56" s="2">
+        <v>2.01E-2</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0.85629999999999995</v>
+      </c>
+      <c r="I56" s="2">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="J56" s="2">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="K56" s="2">
+        <v>1.06E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.71020000000000005</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.66659999999999997</v>
+      </c>
+      <c r="G57" s="2">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="H57" s="2">
+        <v>0.98409999999999997</v>
+      </c>
+      <c r="I57" s="2">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="J57" s="2">
+        <v>0.79479999999999995</v>
+      </c>
+      <c r="K57" s="2">
+        <v>1.44E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.78390000000000004</v>
+      </c>
+      <c r="E58" s="2">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0.74890000000000001</v>
+      </c>
+      <c r="G58" s="2">
+        <v>1.78E-2</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0.93440000000000001</v>
+      </c>
+      <c r="I58" s="2">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="J58" s="2">
+        <v>0.83140000000000003</v>
+      </c>
+      <c r="K58" s="2">
+        <v>1.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="E59" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0.79290000000000005</v>
+      </c>
+      <c r="G59" s="2">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="H59" s="2">
+        <v>0.86460000000000004</v>
+      </c>
+      <c r="I59" s="2">
+        <v>6.3E-3</v>
+      </c>
+      <c r="J59" s="2">
+        <v>0.82709999999999995</v>
+      </c>
+      <c r="K59" s="2">
+        <v>1.0800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0.71779999999999999</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1.67E-2</v>
+      </c>
+      <c r="F60" s="2">
+        <v>0.67359999999999998</v>
+      </c>
+      <c r="G60" s="2">
+        <v>2.06E-2</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0.98070000000000002</v>
+      </c>
+      <c r="I60" s="2">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J60" s="2">
+        <v>0.79849999999999999</v>
+      </c>
+      <c r="K60" s="2">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.78590000000000004</v>
+      </c>
+      <c r="E61" s="2">
+        <v>1.14E-2</v>
+      </c>
+      <c r="F61" s="2">
+        <v>0.75090000000000001</v>
+      </c>
+      <c r="G61" s="2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="H61" s="2">
+        <v>0.93459999999999999</v>
+      </c>
+      <c r="I61" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J61" s="2">
+        <v>0.8327</v>
+      </c>
+      <c r="K61" s="2">
+        <v>1.15E-2</v>
+      </c>
+      <c r="L61" s="1">
+        <v>0.79649999999999999</v>
+      </c>
+      <c r="M61" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D61 E64">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F61">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H61">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J61">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E61">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G61">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I61">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K61">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>